<commit_message>
added 45 for each easy and hard mode
</commit_message>
<xml_diff>
--- a/physiolabxr/scripting/illumiRead/illumiReadSwype/gaze2word/Short_Long_Sentences.xlsx
+++ b/physiolabxr/scripting/illumiRead/illumiReadSwype/gaze2word/Short_Long_Sentences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Season\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Season\Documents\PhysioLab\physiolabxr\scripting\illumiRead\illumiReadSwype\gaze2word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F87EC2-E0C3-4A82-85C0-EA06C2DFCD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F339AD3E-D128-4B74-A9D2-5705D80D39F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{45585804-7EAB-4359-B5A1-5634CDA175BB}"/>
+    <workbookView xWindow="57495" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{45585804-7EAB-4359-B5A1-5634CDA175BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="94">
   <si>
     <t>i can see it in his eyes</t>
   </si>
@@ -157,6 +157,156 @@
   </si>
   <si>
     <t>He ran out into the downpour , sped across the yard and into the buggy room</t>
+  </si>
+  <si>
+    <t>He tried again and once more sliced out of bounds</t>
+  </si>
+  <si>
+    <t>Somebody brought a light</t>
+  </si>
+  <si>
+    <t>The prediction was correct</t>
+  </si>
+  <si>
+    <t>He sized up the situation and shook his head</t>
+  </si>
+  <si>
+    <t>The rancher was trembling</t>
+  </si>
+  <si>
+    <t>The vision became even stronger now</t>
+  </si>
+  <si>
+    <t>He felt a little sick at his stomach</t>
+  </si>
+  <si>
+    <t>His heart beat faster</t>
+  </si>
+  <si>
+    <t>I never heard that</t>
+  </si>
+  <si>
+    <t>Come inside now</t>
+  </si>
+  <si>
+    <t>It was my fault</t>
+  </si>
+  <si>
+    <t>He scarcely saw them</t>
+  </si>
+  <si>
+    <t>Then he smiled shyly</t>
+  </si>
+  <si>
+    <t>His room will be ready shortly</t>
+  </si>
+  <si>
+    <t>The ball broke up in confusion</t>
+  </si>
+  <si>
+    <t>Such a pitiful end</t>
+  </si>
+  <si>
+    <t>That was the day it ended</t>
+  </si>
+  <si>
+    <t>The girl smiled and started forward</t>
+  </si>
+  <si>
+    <t>That was gonna be fun collecting</t>
+  </si>
+  <si>
+    <t>He cleared his throat</t>
+  </si>
+  <si>
+    <t>I been riding train for a ways now</t>
+  </si>
+  <si>
+    <t>This was a slightly different matter</t>
+  </si>
+  <si>
+    <t>Now forget all this other</t>
+  </si>
+  <si>
+    <t>Youth obeyed when commanded</t>
+  </si>
+  <si>
+    <t>But the past was dead here as the present was dead</t>
+  </si>
+  <si>
+    <t>If we wait until children are in junior high or high school , we will never manage it</t>
+  </si>
+  <si>
+    <t>Improvement can be measured by the lessening distance between toes and head</t>
+  </si>
+  <si>
+    <t>He places the hands on either side of the head , keeping the chin down on the chest</t>
+  </si>
+  <si>
+    <t>He then pushes his seat into the air and the teacher guides it over</t>
+  </si>
+  <si>
+    <t>It is very important for parents to understand that early training is imperative</t>
+  </si>
+  <si>
+    <t>This stain often disrupts the normal cell activity or else colors only the outside</t>
+  </si>
+  <si>
+    <t>A balanced resistance bridge and a pen recorder are all the electronic instrumentation needed</t>
+  </si>
+  <si>
+    <t>The transducer is coupled to the body through a water bath , not shown</t>
+  </si>
+  <si>
+    <t>His earlier love for literature and history remained with him for his entire life</t>
+  </si>
+  <si>
+    <t>He proposed a fresh theory of alkalis which later was accepted in chemical practices</t>
+  </si>
+  <si>
+    <t>The form of galvanic activity is halfway between the magnetic form and the electrical form</t>
+  </si>
+  <si>
+    <t>He devised a detonating fuse in which a short wire was caused to glow by an electric current</t>
+  </si>
+  <si>
+    <t>Cows receiving drug may not be officially tested under breed registry testing programs</t>
+  </si>
+  <si>
+    <t>Several materials or combinations of materials can be used to construct a satisfactory feed bunk</t>
+  </si>
+  <si>
+    <t>Here are some key areas to examine to make sure your pricing strategy will be on target</t>
+  </si>
+  <si>
+    <t>This problem can force a change in marketing approach in many kinds of businesses</t>
+  </si>
+  <si>
+    <t>No manufacturer has taken the initiative in pointing out the costs involved</t>
+  </si>
+  <si>
+    <t>Computers are being used to keep branch inventories at more workable levels</t>
+  </si>
+  <si>
+    <t>There may be possible economies at any one of a number of links in your marketing and distribution chain</t>
+  </si>
+  <si>
+    <t>Are there individuals in your organization who can shepherd a new product through to commercialization</t>
+  </si>
+  <si>
+    <t>Most marketing people agree it is going to take redoubled efforts to satisfy future requirements</t>
+  </si>
+  <si>
+    <t>Every single problem touched on thus far is related to good marketing planning</t>
+  </si>
+  <si>
+    <t>Beyond any question of curriculum and approach to subject must be the quality of the teachers themselves</t>
+  </si>
+  <si>
+    <t>Only a few years ago a middle western college circulated a request for a teacher of interior design</t>
+  </si>
+  <si>
+    <t>One solution is the aquisition of degrees in education but it is a poor substitute</t>
   </si>
 </sst>
 </file>
@@ -508,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7164EA21-43E4-4FA1-92B9-CB39328BFC99}">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,21 +830,221 @@
         <v>24</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>37</v>
+      </c>
+      <c r="B120" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>39</v>
       </c>
     </row>

</xml_diff>